<commit_message>
add edit dialog for revenue
</commit_message>
<xml_diff>
--- a/Projects.xlsx
+++ b/Projects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\VUE\Bookeeping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7240CDC-8601-41D0-8820-255C543DDA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91115D0-4800-4074-B908-A1FD1D946F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4410" yWindow="3270" windowWidth="17250" windowHeight="10515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,6 @@
     <t>חלקי 1</t>
   </si>
   <si>
-    <t>קיוסק ת"א</t>
-  </si>
-  <si>
     <t>חלקי 2</t>
   </si>
   <si>
@@ -37,9 +34,6 @@
     <t>סופי</t>
   </si>
   <si>
-    <t>ריז 2 ת"א</t>
-  </si>
-  <si>
     <t>ישרוטל</t>
   </si>
   <si>
@@ -122,6 +116,12 @@
   </si>
   <si>
     <t>project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">קיוסק ת"א </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ריז 2 ת"א </t>
   </si>
 </sst>
 </file>
@@ -990,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,19 +1005,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1034,7 +1034,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1048,10 +1048,10 @@
         <v>5007</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1068,7 +1068,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1082,10 +1082,10 @@
         <v>5009</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1102,7 +1102,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1116,10 +1116,10 @@
         <v>60020</v>
       </c>
       <c r="D7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1133,10 +1133,10 @@
         <v>50013</v>
       </c>
       <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
         <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1150,10 +1150,10 @@
         <v>60021</v>
       </c>
       <c r="D9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1167,10 +1167,10 @@
         <v>80003</v>
       </c>
       <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
         <v>4</v>
-      </c>
-      <c r="E10" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1187,7 +1187,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1201,10 +1201,10 @@
         <v>50014</v>
       </c>
       <c r="D12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1218,10 +1218,10 @@
         <v>50015</v>
       </c>
       <c r="D13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1235,10 +1235,10 @@
         <v>60024</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1252,10 +1252,10 @@
         <v>50018</v>
       </c>
       <c r="D15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1272,7 +1272,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1286,10 +1286,10 @@
         <v>50017</v>
       </c>
       <c r="D17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1303,10 +1303,10 @@
         <v>60028</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1320,10 +1320,10 @@
         <v>60027</v>
       </c>
       <c r="D19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1340,7 +1340,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1354,10 +1354,10 @@
         <v>60031</v>
       </c>
       <c r="D21" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1371,10 +1371,10 @@
         <v>60032</v>
       </c>
       <c r="D22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1391,7 +1391,7 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1408,7 +1408,7 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1425,7 +1425,7 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1439,10 +1439,10 @@
         <v>60035</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1459,7 +1459,7 @@
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1473,10 +1473,10 @@
         <v>60036</v>
       </c>
       <c r="D28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E28" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1490,10 +1490,10 @@
         <v>60037</v>
       </c>
       <c r="D29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1507,10 +1507,10 @@
         <v>50020</v>
       </c>
       <c r="D30" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1524,10 +1524,10 @@
         <v>50021</v>
       </c>
       <c r="D31" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1541,10 +1541,10 @@
         <v>50022</v>
       </c>
       <c r="D32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1558,10 +1558,10 @@
         <v>50023</v>
       </c>
       <c r="D33" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E33" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1575,10 +1575,10 @@
         <v>50025</v>
       </c>
       <c r="D34" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1592,10 +1592,10 @@
         <v>50024</v>
       </c>
       <c r="D35" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E35" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1609,10 +1609,10 @@
         <v>50026</v>
       </c>
       <c r="D36" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E36" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1629,7 +1629,7 @@
         <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1643,10 +1643,10 @@
         <v>50028</v>
       </c>
       <c r="D38" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E38" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1660,10 +1660,10 @@
         <v>50029</v>
       </c>
       <c r="D39" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1677,10 +1677,10 @@
         <v>50030</v>
       </c>
       <c r="D40" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E40" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1694,10 +1694,10 @@
         <v>50031</v>
       </c>
       <c r="D41" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E41" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1711,10 +1711,10 @@
         <v>60038</v>
       </c>
       <c r="D42" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E42" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1728,10 +1728,10 @@
         <v>60038</v>
       </c>
       <c r="D43" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E43" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1748,7 +1748,7 @@
         <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1762,10 +1762,10 @@
         <v>50033</v>
       </c>
       <c r="D45" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1779,10 +1779,10 @@
         <v>50032</v>
       </c>
       <c r="D46" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E46" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1796,10 +1796,10 @@
         <v>50034</v>
       </c>
       <c r="D47" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E47" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1813,10 +1813,10 @@
         <v>50035</v>
       </c>
       <c r="D48" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E48" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1830,10 +1830,10 @@
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E49" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1847,10 +1847,10 @@
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E50" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1867,7 +1867,7 @@
         <v>0</v>
       </c>
       <c r="E51" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1884,7 +1884,7 @@
         <v>0</v>
       </c>
       <c r="E52" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1898,10 +1898,10 @@
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E53" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1915,10 +1915,10 @@
         <v>50036</v>
       </c>
       <c r="D54" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E54" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1932,10 +1932,10 @@
         <v>50038</v>
       </c>
       <c r="D55" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E55" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1949,10 +1949,10 @@
         <v>50037</v>
       </c>
       <c r="D56" t="s">
+        <v>20</v>
+      </c>
+      <c r="E56" t="s">
         <v>22</v>
-      </c>
-      <c r="E56" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1966,10 +1966,10 @@
         <v>60043</v>
       </c>
       <c r="D57" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E57" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>